<commit_message>
Deleted nicole's extra files, added db query file
</commit_message>
<xml_diff>
--- a/C200_Official/wwwroot/ExcelUpload/UploadMember.xlsx
+++ b/C200_Official/wwwroot/ExcelUpload/UploadMember.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\20007073\Desktop\RP\Y2 Sem 2\C200 Special Project\C200_Solution\C200_Offical\C200_Official\wwwroot\ExcelUpload\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\20007073\Desktop\RP\Y2 Sem 2\C200 Special Project\Presentation\V5_C200_Official (2)\C200_Official\wwwroot\ExcelUpload\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{622F47B2-0F35-4BE3-8B3C-6F4B62B97661}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5AF132A-D64F-41DB-97AE-BB24B050C76B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22755" yWindow="2670" windowWidth="14400" windowHeight="7455" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>john_tan</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t>20007073@myrp.edu.sg</t>
+  </si>
+  <si>
+    <t>kijas59503@petloca.com</t>
+  </si>
+  <si>
+    <t>autumnlpx@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -401,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -424,57 +430,87 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C6" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D1" r:id="rId1" xr:uid="{39438444-9B08-4E04-804A-CDD13E3C189B}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{8C247C07-EC90-47F9-AB82-E43BF072E8B7}"/>
-    <hyperlink ref="D3" r:id="rId3" xr:uid="{710BABCD-5A95-42C7-AF95-50D15F57067F}"/>
-    <hyperlink ref="D4" r:id="rId4" xr:uid="{DD89ACBF-25BB-418C-90E6-57D913AE5655}"/>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{39438444-9B08-4E04-804A-CDD13E3C189B}"/>
+    <hyperlink ref="D4" r:id="rId2" xr:uid="{8C247C07-EC90-47F9-AB82-E43BF072E8B7}"/>
+    <hyperlink ref="D5" r:id="rId3" xr:uid="{710BABCD-5A95-42C7-AF95-50D15F57067F}"/>
+    <hyperlink ref="D6" r:id="rId4" xr:uid="{DD89ACBF-25BB-418C-90E6-57D913AE5655}"/>
+    <hyperlink ref="D2" r:id="rId5" xr:uid="{B0356277-0AF4-4272-BE04-56D206A549B0}"/>
+    <hyperlink ref="D1" r:id="rId6" xr:uid="{F9D2C36B-EFC2-40C6-87DE-4964BF546325}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>